<commit_message>
clean up catalogue files, clean up old sim functions, and sim_mvnorm_cl
</commit_message>
<xml_diff>
--- a/apps/study/z_app_variable_map.xlsx
+++ b/apps/study/z_app_variable_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\spinifex_study\apps\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDE9D8E9-E3A4-4A56-A20B-69B67AFB8657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F369D8B-122E-45DE-9C1C-EA3DF520089D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10605" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,15 +799,15 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="57.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5546875" customWidth="1"/>
+    <col min="8" max="8" width="57.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -827,7 +827,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -844,7 +844,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -861,7 +861,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -881,7 +881,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -901,7 +901,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -918,7 +918,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -935,7 +935,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -955,7 +955,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -975,7 +975,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -995,7 +995,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>62</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>63</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>67</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>68</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>71</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>73</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>75</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>76</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>79</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>81</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>83</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>88</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>87</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>86</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>89</v>
       </c>
@@ -1284,27 +1284,27 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H31" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H33" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
sims fixes, loading training, and initial errors, dat() and cl()
</commit_message>
<xml_diff>
--- a/apps/study/z_app_variable_map.xlsx
+++ b/apps/study/z_app_variable_map.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\spinifex_study\apps\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F369D8B-122E-45DE-9C1C-EA3DF520089D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C38B8C-61BF-4AD5-8E18-2A307CD9C463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" activeTab="1" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="app.r" sheetId="1" r:id="rId1"/>
+    <sheet name="simulations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="141">
   <si>
     <t>s_blocks</t>
   </si>
@@ -418,6 +419,36 @@
   </si>
   <si>
     <t>reactive values, see table to the right</t>
+  </si>
+  <si>
+    <t>baseLn_EEE.rda</t>
+  </si>
+  <si>
+    <t>baseLn_EEV.rda</t>
+  </si>
+  <si>
+    <t>baseLn_banana.rda</t>
+  </si>
+  <si>
+    <t>corNoise_EEE.rda</t>
+  </si>
+  <si>
+    <t>corNoise_EEV.rda</t>
+  </si>
+  <si>
+    <t>corNoise_banana.rda</t>
+  </si>
+  <si>
+    <t>mnComb_EEE.rda</t>
+  </si>
+  <si>
+    <t>mnComb_EEV.rda</t>
+  </si>
+  <si>
+    <t>mnComb_banana.rda</t>
+  </si>
+  <si>
+    <t>filenames in "apps/data/"</t>
   </si>
 </sst>
 </file>
@@ -470,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -479,6 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6878FC98-F4AF-4AE1-84C9-16578B92340E}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1313,4 +1345,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAA3EA-3E77-4C76-9318-A8F9464C946D}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data .rds to .rda, geneerate and save tpaths.
</commit_message>
<xml_diff>
--- a/apps/study/z_app_variable_map.xlsx
+++ b/apps/study/z_app_variable_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\spinifex_study\apps\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C38B8C-61BF-4AD5-8E18-2A307CD9C463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C78CF5-1744-4ED3-823C-FB24CC4943F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" activeTab="1" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
   </bookViews>
@@ -421,34 +421,34 @@
     <t>reactive values, see table to the right</t>
   </si>
   <si>
-    <t>baseLn_EEE.rda</t>
-  </si>
-  <si>
-    <t>baseLn_EEV.rda</t>
-  </si>
-  <si>
-    <t>baseLn_banana.rda</t>
-  </si>
-  <si>
-    <t>corNoise_EEE.rda</t>
-  </si>
-  <si>
-    <t>corNoise_EEV.rda</t>
-  </si>
-  <si>
-    <t>corNoise_banana.rda</t>
-  </si>
-  <si>
-    <t>mnComb_EEE.rda</t>
-  </si>
-  <si>
-    <t>mnComb_EEV.rda</t>
-  </si>
-  <si>
-    <t>mnComb_banana.rda</t>
-  </si>
-  <si>
     <t>filenames in "apps/data/"</t>
+  </si>
+  <si>
+    <t>baseLn_EEE.rds</t>
+  </si>
+  <si>
+    <t>baseLn_EEV.rds</t>
+  </si>
+  <si>
+    <t>baseLn_banana.rds</t>
+  </si>
+  <si>
+    <t>corNoise_EEE.rds</t>
+  </si>
+  <si>
+    <t>corNoise_EEV.rds</t>
+  </si>
+  <si>
+    <t>corNoise_banana.rds</t>
+  </si>
+  <si>
+    <t>mnComb_EEE.rds</t>
+  </si>
+  <si>
+    <t>mnComb_EEV.rds</t>
+  </si>
+  <si>
+    <t>mnComb_banana.rds</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,52 +1362,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gutting app, is stable at least.
</commit_message>
<xml_diff>
--- a/apps/study/z_app_variable_map.xlsx
+++ b/apps/study/z_app_variable_map.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\spinifex_study\apps\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C78CF5-1744-4ED3-823C-FB24CC4943F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351A79C2-DF5C-41ED-A1F1-0797EABC0714}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" activeTab="1" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
   </bookViews>
   <sheets>
     <sheet name="app.r" sheetId="1" r:id="rId1"/>
-    <sheet name="simulations" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="simulations" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="195">
   <si>
     <t>s_blocks</t>
   </si>
@@ -112,18 +113,12 @@
     <t>rv</t>
   </si>
   <si>
-    <t>rv$pg</t>
-  </si>
-  <si>
     <t>period</t>
   </si>
   <si>
     <t>desp</t>
   </si>
   <si>
-    <t>integer of curr page</t>
-  </si>
-  <si>
     <t>name of section</t>
   </si>
   <si>
@@ -449,13 +444,181 @@
   </si>
   <si>
     <t>mnComb_banana.rds</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>section pg</t>
+  </si>
+  <si>
+    <t>section nm</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Eval</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VC </t>
+  </si>
+  <si>
+    <t>#var (cl)</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Sim name</t>
+  </si>
+  <si>
+    <t>Grand path</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Grand</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>4v (3cl)</t>
+  </si>
+  <si>
+    <t>33_66</t>
+  </si>
+  <si>
+    <t>EEE_p4_0_1_t1</t>
+  </si>
+  <si>
+    <t>tpath_p4_t</t>
+  </si>
+  <si>
+    <t>1_0</t>
+  </si>
+  <si>
+    <t>EEE_p4_50_50_rep1</t>
+  </si>
+  <si>
+    <t>tpath_p4</t>
+  </si>
+  <si>
+    <t>6v in (4cl)</t>
+  </si>
+  <si>
+    <t>EEE_p6_50_50_rep1</t>
+  </si>
+  <si>
+    <t>tpath_p6</t>
+  </si>
+  <si>
+    <t>Radial</t>
+  </si>
+  <si>
+    <t>EEE_p4_0_1_t2</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>EEV_p4_50_50_rep1</t>
+  </si>
+  <si>
+    <t>EEV_p6_50_50_rep2</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>EEE_p4_0_1_t3</t>
+  </si>
+  <si>
+    <t>banana_p4_50_50_rep3</t>
+  </si>
+  <si>
+    <t>banana_p6_50_50_rep3</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>study structure</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>intermission</t>
+  </si>
+  <si>
+    <t>period1</t>
+  </si>
+  <si>
+    <t>period2</t>
+  </si>
+  <si>
+    <t>period3</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI </t>
+  </si>
+  <si>
+    <t>blue/green</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>response table</t>
+  </si>
+  <si>
+    <t>participant_num</t>
+  </si>
+  <si>
+    <t>ttr</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+  <si>
+    <t>full perm_num</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>interations</t>
+  </si>
+  <si>
+    <t>survey questions</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,16 +634,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EBF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFD5EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -497,11 +723,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,6 +782,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,14 +1130,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6878FC98-F4AF-4AE1-84C9-16578B92340E}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
     <col min="6" max="6" width="47.5546875" customWidth="1"/>
     <col min="8" max="8" width="57.44140625" customWidth="1"/>
   </cols>
@@ -853,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -870,10 +1175,10 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -883,14 +1188,9 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -904,13 +1204,13 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -924,13 +1224,13 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -941,13 +1241,13 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -958,13 +1258,13 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -975,16 +1275,16 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -995,16 +1295,16 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1015,16 +1315,16 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1035,16 +1335,16 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1055,16 +1355,16 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
         <v>51</v>
       </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
       <c r="H12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1075,16 +1375,16 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1095,16 +1395,16 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
         <v>57</v>
       </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1115,230 +1415,230 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
-      </c>
       <c r="H16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" t="s">
-        <v>65</v>
-      </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="F18" t="s">
-        <v>69</v>
-      </c>
       <c r="H18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" t="s">
         <v>68</v>
       </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
         <v>75</v>
       </c>
-      <c r="F22" t="s">
-        <v>77</v>
-      </c>
       <c r="H22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="F23" t="s">
-        <v>78</v>
-      </c>
       <c r="H23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" t="s">
         <v>83</v>
       </c>
-      <c r="E26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="s">
-        <v>85</v>
-      </c>
       <c r="H26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" t="s">
-        <v>90</v>
-      </c>
       <c r="H27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1648,967 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89093FA4-2388-4A93-8284-B5811C6DC37A}">
+  <dimension ref="A1:U26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:R16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="19" width="9.109375" customWidth="1"/>
+    <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>165</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" t="s">
+        <v>165</v>
+      </c>
+      <c r="M3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="T3" t="s">
+        <v>183</v>
+      </c>
+      <c r="U3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s">
+        <v>165</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" t="s">
+        <v>165</v>
+      </c>
+      <c r="L4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="T4" t="s">
+        <v>182</v>
+      </c>
+      <c r="U4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K8" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" t="s">
+        <v>165</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="11">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11">
+        <v>3</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="R10" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" t="s">
+        <v>165</v>
+      </c>
+      <c r="J12" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" t="s">
+        <v>165</v>
+      </c>
+      <c r="L12" t="s">
+        <v>165</v>
+      </c>
+      <c r="M12" t="s">
+        <v>165</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="8">
+        <v>3</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>5</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="P14" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q14" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="R14" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="11">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11">
+        <v>6</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="R15" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" t="s">
+        <v>165</v>
+      </c>
+      <c r="K16" t="s">
+        <v>165</v>
+      </c>
+      <c r="L16" t="s">
+        <v>165</v>
+      </c>
+      <c r="M16" t="s">
+        <v>165</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CAA3EA-3E77-4C76-9318-A8F9464C946D}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1362,52 +2619,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
png/gif, saving script grand still not working; interpolate(): err; Fa not tourr::is_orthonormal (scalar number);
</commit_message>
<xml_diff>
--- a/apps/study/z_app_variable_map.xlsx
+++ b/apps/study/z_app_variable_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Spyrison\Documents\R\spinifex_study\apps\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961DC8AB-023C-4FA3-87DC-5B3759D54446}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DD1A3-DCDA-4807-93E2-BCCE42441F6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10608" activeTab="1" xr2:uid="{DF5B416B-9777-4CBF-9A96-5671FCA6F72A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="195">
   <si>
     <t>s_blocks</t>
   </si>
@@ -476,9 +476,6 @@
     <t>Sim name</t>
   </si>
   <si>
-    <t>Grand path</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
@@ -491,18 +488,12 @@
     <t>4v (3cl)</t>
   </si>
   <si>
-    <t>33_66</t>
-  </si>
-  <si>
     <t>EEE_p4_0_1_t1</t>
   </si>
   <si>
     <t>tpath_p4_t</t>
   </si>
   <si>
-    <t>1_0</t>
-  </si>
-  <si>
     <t>EEE_p4_50_50_rep1</t>
   </si>
   <si>
@@ -527,24 +518,12 @@
     <t>NA</t>
   </si>
   <si>
-    <t>EEV_p4_50_50_rep1</t>
-  </si>
-  <si>
-    <t>EEV_p6_50_50_rep2</t>
-  </si>
-  <si>
     <t>PCA</t>
   </si>
   <si>
     <t>EEE_p4_0_1_t3</t>
   </si>
   <si>
-    <t>banana_p4_50_50_rep3</t>
-  </si>
-  <si>
-    <t>banana_p6_50_50_rep3</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
@@ -584,9 +563,6 @@
     <t>response table</t>
   </si>
   <si>
-    <t>participant_num</t>
-  </si>
-  <si>
     <t>ttr</t>
   </si>
   <si>
@@ -599,19 +575,43 @@
     <t>marks</t>
   </si>
   <si>
-    <t>full perm_num</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
-    <t>interations</t>
-  </si>
-  <si>
     <t>survey questions</t>
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Image name</t>
+  </si>
+  <si>
+    <t>Grand path  name</t>
+  </si>
+  <si>
+    <t>control interations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response interactions </t>
+  </si>
+  <si>
+    <t>0_1</t>
+  </si>
+  <si>
+    <t>50_50</t>
+  </si>
+  <si>
+    <t>EEE_p4_0_1_rep1</t>
+  </si>
+  <si>
+    <t>EEE_p6_0_1_rep1</t>
+  </si>
+  <si>
+    <t>participant num</t>
+  </si>
+  <si>
+    <t>full perm num</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -664,7 +664,7 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -708,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -748,7 +748,22 @@
         <color rgb="FFFFFFFF"/>
       </right>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color rgb="FFFFFFFF"/>
@@ -763,6 +778,36 @@
         <color rgb="FFFFFFFF"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
         <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="medium">
@@ -770,11 +815,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -787,34 +892,71 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1651,49 +1793,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89093FA4-2388-4A93-8284-B5811C6DC37A}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
     <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" customWidth="1"/>
-    <col min="18" max="19" width="9.109375" customWidth="1"/>
-    <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
+    <col min="20" max="21" width="9.109375" customWidth="1"/>
+    <col min="22" max="22" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="D1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" t="s">
-        <v>190</v>
+      <c r="D1" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>194</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>142</v>
@@ -1717,877 +1862,955 @@
         <v>148</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="19">
+        <v>1</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="19">
+        <v>0</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="19">
+        <v>0</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="V3" t="s">
+        <v>176</v>
+      </c>
+      <c r="W3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="19">
+        <v>1</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="V4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="H5" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="R5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19">
+        <v>2</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="T6" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19">
+        <v>3</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="19">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15">
+        <v>2</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="T7" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <v>4</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="19">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T8" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19">
+        <v>1</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="19">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="T9" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="16">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="O10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="P10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="R10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="S10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="T10" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19">
+        <v>3</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="19">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18">
+        <v>4</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="L11" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="R1" s="7" t="s">
+      <c r="M11" s="18"/>
+      <c r="N11" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="O11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="P11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="T11" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="19">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="19">
+        <v>2</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S12" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T12" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="19">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="11">
+        <v>3</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="L13" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="T13" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19">
+        <v>2</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="19">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="E14" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3</v>
+      </c>
+      <c r="G14" s="8">
+        <v>5</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="R14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="S14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="T14" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="19">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19">
+        <v>3</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="19">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E15" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="14">
+        <v>3</v>
+      </c>
+      <c r="G15" s="15">
+        <v>6</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="O15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="R15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="S15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="T15" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="D2">
+      <c r="D16" s="19">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J2" t="s">
-        <v>165</v>
-      </c>
-      <c r="K2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M2" t="s">
-        <v>165</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J3" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" t="s">
-        <v>165</v>
-      </c>
-      <c r="L3" t="s">
-        <v>165</v>
-      </c>
-      <c r="M3" t="s">
-        <v>165</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="E16" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="19">
+        <v>4</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="U3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" t="s">
-        <v>165</v>
-      </c>
-      <c r="J4" t="s">
-        <v>165</v>
-      </c>
-      <c r="K4" t="s">
-        <v>165</v>
-      </c>
-      <c r="L4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M4" t="s">
-        <v>165</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="T4" t="s">
-        <v>182</v>
-      </c>
-      <c r="U4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10">
-        <v>2</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q7" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="R7" s="17" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>175</v>
-      </c>
-      <c r="H8" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L8" t="s">
-        <v>165</v>
-      </c>
-      <c r="M8" t="s">
-        <v>165</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q8" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R8" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="8">
-        <v>2</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="P9" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q9" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="11">
-        <v>2</v>
-      </c>
-      <c r="G10" s="11">
-        <v>3</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="O10" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="P10" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q10" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F11" s="12">
-        <v>2</v>
-      </c>
-      <c r="G11" s="12">
-        <v>4</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q11" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>191</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" t="s">
-        <v>165</v>
-      </c>
-      <c r="I12" t="s">
-        <v>165</v>
-      </c>
-      <c r="J12" t="s">
-        <v>165</v>
-      </c>
-      <c r="K12" t="s">
-        <v>165</v>
-      </c>
-      <c r="L12" t="s">
-        <v>165</v>
-      </c>
-      <c r="M12" t="s">
-        <v>165</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R12" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="8">
-        <v>3</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q13" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="R13" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>191</v>
-      </c>
-      <c r="F14" s="9">
-        <v>3</v>
-      </c>
-      <c r="G14" s="9">
-        <v>5</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q14" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F15" s="11">
-        <v>3</v>
-      </c>
-      <c r="G15" s="11">
-        <v>6</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="N15" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="O15" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="P15" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q15" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="R15" s="17" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>191</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>193</v>
-      </c>
-      <c r="H16" t="s">
-        <v>165</v>
-      </c>
-      <c r="I16" t="s">
-        <v>165</v>
-      </c>
-      <c r="J16" t="s">
-        <v>165</v>
-      </c>
-      <c r="K16" t="s">
-        <v>165</v>
-      </c>
-      <c r="L16" t="s">
-        <v>165</v>
-      </c>
-      <c r="M16" t="s">
-        <v>165</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="R16" s="14" t="s">
-        <v>165</v>
+      <c r="H16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="R16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="S16" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="T16" s="20" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>